<commit_message>
Expansion of the plotting script to plot the B2
</commit_message>
<xml_diff>
--- a/aux_info/DG_amino_acids.xlsx
+++ b/aux_info/DG_amino_acids.xlsx
@@ -33,6 +33,7 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Not reported, I copied the value from the Lys</t>
         </r>
@@ -164,7 +165,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -194,12 +195,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -275,7 +270,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -284,7 +279,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -300,10 +295,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -316,10 +307,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -332,7 +319,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -419,8 +406,8 @@
   </sheetPr>
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H25" activeCellId="0" sqref="H25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -428,9 +415,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.74"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="8.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.89"/>
   </cols>
@@ -458,10 +445,10 @@
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6" t="n">
+      <c r="B2" s="2" t="n">
         <v>0.4</v>
       </c>
-      <c r="C2" s="6" t="n">
+      <c r="C2" s="2" t="n">
         <f aca="false">LN(10)*$B$32*$B$31*B2</f>
         <v>2243.76543337495</v>
       </c>
@@ -472,64 +459,64 @@
         <f aca="false">D2/C2</f>
         <v>0.0800440176716046</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="8" t="n">
+      <c r="B3" s="7" t="n">
         <v>-0.12</v>
       </c>
-      <c r="C3" s="6" t="n">
+      <c r="C3" s="2" t="n">
         <f aca="false">LN(10)*$B$32*$B$31*B3</f>
         <v>-673.129630012486</v>
       </c>
-      <c r="D3" s="9" t="n">
+      <c r="D3" s="8" t="n">
         <v>321.833333333333</v>
       </c>
-      <c r="E3" s="10" t="n">
+      <c r="E3" s="5" t="n">
         <f aca="false">D3/C3</f>
         <v>-0.47811494099192</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="6"/>
       <c r="G3" s="5"/>
-      <c r="H3" s="6"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B4" s="2" t="n">
         <v>-0.9</v>
       </c>
-      <c r="C4" s="6" t="n">
+      <c r="C4" s="2" t="n">
         <f aca="false">LN(10)*$B$32*$B$31*B4</f>
         <v>-5048.47222509364</v>
       </c>
-      <c r="D4" s="9" t="n">
+      <c r="D4" s="8" t="n">
         <v>321.833333333333</v>
       </c>
       <c r="E4" s="5" t="n">
         <f aca="false">D4/C4</f>
         <v>-0.0637486587989228</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="6"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="6"/>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="6" t="n">
+      <c r="B5" s="2" t="n">
         <v>-0.16</v>
       </c>
-      <c r="C5" s="6" t="n">
+      <c r="C5" s="2" t="n">
         <f aca="false">LN(10)*$B$32*$B$31*B5</f>
         <v>-897.506173349981</v>
       </c>
@@ -540,18 +527,18 @@
         <f aca="false">D5/C5</f>
         <v>-0.146702797792705</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="6"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="6"/>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="6" t="n">
+      <c r="B6" s="2" t="n">
         <v>-0.07</v>
       </c>
-      <c r="C6" s="6" t="n">
+      <c r="C6" s="2" t="n">
         <f aca="false">LN(10)*$B$32*$B$31*B6</f>
         <v>-392.658950840617</v>
       </c>
@@ -562,18 +549,18 @@
         <f aca="false">D6/C6</f>
         <v>-0.331840136895007</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="6"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="6"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="6" t="n">
+      <c r="B7" s="2" t="n">
         <v>-1.05</v>
       </c>
-      <c r="C7" s="6" t="n">
+      <c r="C7" s="2" t="n">
         <f aca="false">LN(10)*$B$32*$B$31*B7</f>
         <v>-5889.88426260925</v>
       </c>
@@ -584,18 +571,18 @@
         <f aca="false">D7/C7</f>
         <v>-0.0221226757930005</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="6"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="6"/>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="6" t="n">
+      <c r="B8" s="2" t="n">
         <v>0.82</v>
       </c>
-      <c r="C8" s="6" t="n">
+      <c r="C8" s="2" t="n">
         <f aca="false">LN(10)*$B$32*$B$31*B8</f>
         <v>4599.71913841865</v>
       </c>
@@ -606,18 +593,18 @@
         <f aca="false">D8/C8</f>
         <v>0.0594456585510865</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="6"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="6" t="n">
+      <c r="B9" s="2" t="n">
         <v>-0.39</v>
       </c>
-      <c r="C9" s="6" t="n">
+      <c r="C9" s="2" t="n">
         <f aca="false">LN(10)*$B$32*$B$31*B9</f>
         <v>-2187.67129754058</v>
       </c>
@@ -628,40 +615,40 @@
         <f aca="false">D9/C9</f>
         <v>-0.124988307722797</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="6"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="6"/>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="6" t="n">
+      <c r="B10" s="2" t="n">
         <v>0.1</v>
       </c>
-      <c r="C10" s="6" t="n">
+      <c r="C10" s="2" t="n">
         <f aca="false">LN(10)*$B$32*$B$31*B10</f>
         <v>560.941358343738</v>
       </c>
       <c r="D10" s="5" t="n">
         <v>216.033333333333</v>
       </c>
-      <c r="E10" s="10" t="n">
+      <c r="E10" s="5" t="n">
         <f aca="false">D10/C10</f>
         <v>0.385126413162337</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="6"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="6"/>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="6" t="n">
+      <c r="B11" s="2" t="n">
         <v>0.36</v>
       </c>
-      <c r="C11" s="6" t="n">
+      <c r="C11" s="2" t="n">
         <f aca="false">LN(10)*$B$32*$B$31*B11</f>
         <v>2019.38889003746</v>
       </c>
@@ -672,40 +659,40 @@
         <f aca="false">D11/C11</f>
         <v>0.106616413045635</v>
       </c>
-      <c r="F11" s="7"/>
+      <c r="F11" s="6"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="6"/>
+      <c r="H11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="6" t="n">
+      <c r="B12" s="2" t="n">
         <v>-0.98</v>
       </c>
-      <c r="C12" s="6" t="n">
+      <c r="C12" s="2" t="n">
         <f aca="false">LN(10)*$B$32*$B$31*B12</f>
         <v>-5497.22531176863</v>
       </c>
       <c r="D12" s="5" t="n">
         <v>215.3</v>
       </c>
-      <c r="E12" s="10" t="n">
+      <c r="E12" s="5" t="n">
         <f aca="false">D12/C12</f>
         <v>-0.0391652129555394</v>
       </c>
-      <c r="F12" s="7"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="6"/>
+      <c r="H12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="6" t="n">
+      <c r="B13" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="C13" s="6" t="n">
+      <c r="C13" s="2" t="n">
         <f aca="false">LN(10)*$B$32*$B$31*B13</f>
         <v>0</v>
       </c>
@@ -713,18 +700,18 @@
         <v>95.7666666666667</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="7"/>
+      <c r="F13" s="6"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="6"/>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="6" t="n">
+      <c r="B14" s="2" t="n">
         <v>0.39</v>
       </c>
-      <c r="C14" s="6" t="n">
+      <c r="C14" s="2" t="n">
         <f aca="false">LN(10)*$B$32*$B$31*B14</f>
         <v>2187.67129754058</v>
       </c>
@@ -735,191 +722,191 @@
         <f aca="false">D14/C14</f>
         <v>0.0925794170088645</v>
       </c>
-      <c r="F14" s="7"/>
+      <c r="F14" s="6"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="6"/>
+      <c r="H14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="7" t="n">
+      <c r="B15" s="6" t="n">
         <v>-0.84</v>
       </c>
-      <c r="C15" s="6" t="n">
+      <c r="C15" s="2" t="n">
         <f aca="false">LN(10)*$B$32*$B$31*B15</f>
         <v>-4711.9074100874</v>
       </c>
       <c r="D15" s="5" t="n">
         <v>202.533333333333</v>
       </c>
-      <c r="E15" s="10" t="n">
+      <c r="E15" s="5" t="n">
         <f aca="false">D15/C15</f>
         <v>-0.0429833007541157</v>
       </c>
-      <c r="F15" s="7"/>
+      <c r="F15" s="6"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="6"/>
+      <c r="H15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="6" t="n">
+      <c r="B16" s="2" t="n">
         <v>1.55</v>
       </c>
-      <c r="C16" s="6" t="n">
+      <c r="C16" s="2" t="n">
         <f aca="false">LN(10)*$B$32*$B$31*B16</f>
         <v>8694.59105432794</v>
       </c>
       <c r="D16" s="5" t="n">
         <v>420.466666666667</v>
       </c>
-      <c r="E16" s="11" t="n">
+      <c r="E16" s="9" t="n">
         <f aca="false">D16/C16</f>
         <v>0.0483595679244016</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G16" s="5"/>
-      <c r="H16" s="6"/>
+      <c r="H16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="6" t="n">
+      <c r="B17" s="2" t="n">
         <v>1.64</v>
       </c>
-      <c r="C17" s="6" t="n">
+      <c r="C17" s="2" t="n">
         <f aca="false">LN(10)*$B$32*$B$31*B17</f>
         <v>9199.4382768373</v>
       </c>
       <c r="D17" s="5" t="n">
         <v>401.2</v>
       </c>
-      <c r="E17" s="11" t="n">
+      <c r="E17" s="9" t="n">
         <f aca="false">D17/C17</f>
         <v>0.04361135842502</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G17" s="5"/>
-      <c r="H17" s="6"/>
+      <c r="H17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="6" t="n">
+      <c r="B18" s="2" t="n">
         <v>-0.12</v>
       </c>
-      <c r="C18" s="6" t="n">
+      <c r="C18" s="2" t="n">
         <f aca="false">LN(10)*$B$32*$B$31*B18</f>
         <v>-673.129630012486</v>
       </c>
       <c r="D18" s="5" t="n">
         <v>287.433333333333</v>
       </c>
-      <c r="E18" s="10" t="n">
+      <c r="E18" s="5" t="n">
         <f aca="false">D18/C18</f>
         <v>-0.427010371431728</v>
       </c>
-      <c r="F18" s="7"/>
+      <c r="F18" s="6"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="6"/>
+      <c r="H18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="6" t="n">
+      <c r="B19" s="2" t="n">
         <v>-1.14</v>
       </c>
-      <c r="C19" s="6" t="n">
+      <c r="C19" s="2" t="n">
         <f aca="false">LN(10)*$B$32*$B$31*B19</f>
         <v>-6394.73148511861</v>
       </c>
       <c r="D19" s="5" t="n">
         <v>287.433333333333</v>
       </c>
-      <c r="E19" s="10" t="n">
+      <c r="E19" s="5" t="n">
         <f aca="false">D19/C19</f>
         <v>-0.0449484601507082</v>
       </c>
-      <c r="F19" s="7"/>
+      <c r="F19" s="6"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="6"/>
+      <c r="H19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="6" t="n">
+      <c r="B20" s="2" t="n">
         <v>1.42</v>
       </c>
-      <c r="C20" s="6" t="n">
+      <c r="C20" s="2" t="n">
         <f aca="false">LN(10)*$B$32*$B$31*B20</f>
         <v>7965.36728848108</v>
       </c>
       <c r="D20" s="5" t="n">
         <v>186.366666666667</v>
       </c>
-      <c r="E20" s="12" t="n">
+      <c r="E20" s="10" t="n">
         <f aca="false">D20/C20</f>
         <v>0.0233971215534752</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G20" s="5"/>
-      <c r="H20" s="6"/>
+      <c r="H20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="6" t="n">
+      <c r="B21" s="2" t="n">
         <v>1.63</v>
       </c>
-      <c r="C21" s="6" t="n">
+      <c r="C21" s="2" t="n">
         <f aca="false">LN(10)*$B$32*$B$31*B21</f>
         <v>9143.34414100293</v>
       </c>
       <c r="D21" s="5" t="n">
         <v>394.3</v>
       </c>
-      <c r="E21" s="11" t="n">
+      <c r="E21" s="9" t="n">
         <f aca="false">D21/C21</f>
         <v>0.043124265467793</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G21" s="5"/>
-      <c r="H21" s="6"/>
+      <c r="H21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="6" t="n">
+      <c r="B22" s="2" t="n">
         <v>0.77</v>
       </c>
-      <c r="C22" s="6" t="n">
+      <c r="C22" s="2" t="n">
         <f aca="false">LN(10)*$B$32*$B$31*B22</f>
         <v>4319.24845924678</v>
       </c>
       <c r="D22" s="5" t="n">
         <v>181.333333333333</v>
       </c>
-      <c r="E22" s="11" t="n">
+      <c r="E22" s="9" t="n">
         <f aca="false">D22/C22</f>
         <v>0.0419826122632814</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G22" s="5"/>
@@ -928,10 +915,10 @@
       <c r="A23" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="6" t="n">
+      <c r="B23" s="2" t="n">
         <v>-0.08</v>
       </c>
-      <c r="C23" s="6" t="n">
+      <c r="C23" s="2" t="n">
         <f aca="false">LN(10)*$B$32*$B$31*B23</f>
         <v>-448.75308667499</v>
       </c>
@@ -942,17 +929,17 @@
         <f aca="false">D23/C23</f>
         <v>-0.245049382237031</v>
       </c>
-      <c r="F23" s="7"/>
+      <c r="F23" s="6"/>
       <c r="G23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="6" t="n">
+      <c r="B24" s="2" t="n">
         <v>0.33</v>
       </c>
-      <c r="C24" s="6" t="n">
+      <c r="C24" s="2" t="n">
         <f aca="false">LN(10)*$B$32*$B$31*B24</f>
         <v>1851.10648253434</v>
       </c>
@@ -963,28 +950,28 @@
         <f aca="false">D24/C24</f>
         <v>0.112545299419029</v>
       </c>
-      <c r="F24" s="7"/>
+      <c r="F24" s="6"/>
       <c r="G24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="6" t="n">
+      <c r="B25" s="2" t="n">
         <v>1.14</v>
       </c>
-      <c r="C25" s="6" t="n">
+      <c r="C25" s="2" t="n">
         <f aca="false">LN(10)*$B$32*$B$31*B25</f>
         <v>6394.73148511861</v>
       </c>
       <c r="D25" s="5" t="n">
         <v>469.8</v>
       </c>
-      <c r="E25" s="12" t="n">
+      <c r="E25" s="10" t="n">
         <f aca="false">D25/C25</f>
         <v>0.073466728211073</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G25" s="5"/>
@@ -993,10 +980,10 @@
       <c r="A26" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="6" t="n">
+      <c r="B26" s="2" t="n">
         <v>0.88</v>
       </c>
-      <c r="C26" s="6" t="n">
+      <c r="C26" s="2" t="n">
         <f aca="false">LN(10)*$B$32*$B$31*B26</f>
         <v>4936.2839534249</v>
       </c>
@@ -1007,35 +994,35 @@
         <f aca="false">D26/C26</f>
         <v>0.0650016631324547</v>
       </c>
-      <c r="F26" s="7"/>
+      <c r="F26" s="6"/>
       <c r="G26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="6" t="n">
+      <c r="B27" s="2" t="n">
         <v>1.18</v>
       </c>
-      <c r="C27" s="6" t="n">
+      <c r="C27" s="2" t="n">
         <f aca="false">LN(10)*$B$32*$B$31*B27</f>
         <v>6619.10802845611</v>
       </c>
       <c r="D27" s="5" t="n">
         <v>328.733333333333</v>
       </c>
-      <c r="E27" s="11" t="n">
+      <c r="E27" s="9" t="n">
         <f aca="false">D27/C27</f>
         <v>0.0496642949352209</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
@@ -1044,18 +1031,21 @@
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
-      <c r="E29" s="13" t="n">
+      <c r="E29" s="11" t="n">
         <f aca="false">AVERAGE(E2,E16,E17,E20,E21,E22,E25,E27)</f>
         <v>0.0504562458064837</v>
       </c>
-      <c r="F29" s="7"/>
+      <c r="F29" s="6" t="n">
+        <f aca="false">E29/2</f>
+        <v>0.0252281229032419</v>
+      </c>
       <c r="G29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E30" s="14" t="n">
+      <c r="E30" s="12" t="n">
         <f aca="false">STDEV(E2,E16,E17,E20,E21,E22,E25,E27)</f>
         <v>0.0181837874354137</v>
       </c>
@@ -1064,7 +1054,7 @@
       <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="15" t="n">
+      <c r="B31" s="13" t="n">
         <v>293</v>
       </c>
       <c r="C31" s="1" t="s">

</xml_diff>

<commit_message>
Add new set of value for DeltaG of aa solvation from another source which give similar slope values to Hackan paper
</commit_message>
<xml_diff>
--- a/aux_info/DG_amino_acids.xlsx
+++ b/aux_info/DG_amino_acids.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t xml:space="preserve">Residue</t>
   </si>
@@ -52,7 +52,7 @@
     <t xml:space="preserve">log10(K) uncharged</t>
   </si>
   <si>
-    <t xml:space="preserve">DeltaG [J/mol]</t>
+    <t xml:space="preserve">DeltaG [J/mol] (Ref. A)</t>
   </si>
   <si>
     <t xml:space="preserve">DeltaCp [J/K/mol]</t>
@@ -61,6 +61,15 @@
     <t xml:space="preserve">DeltaCp/DeltaG [1/K]</t>
   </si>
   <si>
+    <t xml:space="preserve">DeltaG [Kcal/mol] (Ref. B)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">corrected by size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J/mol</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ala</t>
   </si>
   <si>
@@ -142,19 +151,25 @@
     <t xml:space="preserve">Val</t>
   </si>
   <si>
+    <t xml:space="preserve">Conv Kcal to J</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T [K]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not sure but I assumed it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R [J/mol/K]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reference:</t>
   </si>
   <si>
-    <t xml:space="preserve">10.1016/S0021-9673(00)82337-7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T [K]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not sure but I assumed it</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R [J/mol/K]</t>
+    <t xml:space="preserve">A) 10.1016/S0021-9673(00)82337-7 (VLADIMIR PLISKA*, MANFRED SCHMIDT and JEAN-LUC FAUCHl?RE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B) https://doi.org/10.1021/bi00104a017 (    Kim A. SharpAnthony NichollsRichard FriedmanBarry Honig)</t>
   </si>
 </sst>
 </file>
@@ -404,22 +419,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="N32" activeCellId="0" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="17.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="25.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="20.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="21.04"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -439,17 +461,34 @@
         <v>4</v>
       </c>
       <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="G1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="C2" s="2" t="n">
-        <f aca="false">LN(10)*$B$32*$B$31*B2</f>
+        <f aca="false">LN(10)*$B$33*$B$32*B2</f>
         <v>2243.76543337495</v>
       </c>
       <c r="D2" s="5" t="n">
@@ -457,23 +496,51 @@
       </c>
       <c r="E2" s="5" t="n">
         <f aca="false">D2/C2</f>
-        <v>0.0800440176716046</v>
+        <v>0.0800440176716045</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>2.89</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <f aca="false">G2-$G$13</f>
+        <v>0.87</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <f aca="false">H2-$H$13</f>
+        <v>1.42</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <f aca="false">I2*$G$32</f>
+        <v>3608.76</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <f aca="false">J2*$G$32</f>
+        <v>5890.16</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <f aca="false">$D$2/K2</f>
+        <v>0.0497677872731908</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <f aca="false">$D$2/L2</f>
+        <v>0.0304915316392084</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>-0.12</v>
       </c>
       <c r="C3" s="2" t="n">
-        <f aca="false">LN(10)*$B$32*$B$31*B3</f>
+        <f aca="false">LN(10)*$B$33*$B$32*B3</f>
         <v>-673.129630012486</v>
       </c>
       <c r="D3" s="8" t="n">
@@ -481,21 +548,21 @@
       </c>
       <c r="E3" s="5" t="n">
         <f aca="false">D3/C3</f>
-        <v>-0.47811494099192</v>
+        <v>-0.478114940991921</v>
       </c>
       <c r="F3" s="6"/>
-      <c r="G3" s="5"/>
+      <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>-0.9</v>
       </c>
       <c r="C4" s="2" t="n">
-        <f aca="false">LN(10)*$B$32*$B$31*B4</f>
+        <f aca="false">LN(10)*$B$33*$B$32*B4</f>
         <v>-5048.47222509364</v>
       </c>
       <c r="D4" s="8" t="n">
@@ -506,18 +573,18 @@
         <v>-0.0637486587989228</v>
       </c>
       <c r="F4" s="6"/>
-      <c r="G4" s="5"/>
+      <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>-0.16</v>
       </c>
       <c r="C5" s="2" t="n">
-        <f aca="false">LN(10)*$B$32*$B$31*B5</f>
+        <f aca="false">LN(10)*$B$33*$B$32*B5</f>
         <v>-897.506173349981</v>
       </c>
       <c r="D5" s="5" t="n">
@@ -528,18 +595,18 @@
         <v>-0.146702797792705</v>
       </c>
       <c r="F5" s="6"/>
-      <c r="G5" s="5"/>
+      <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>-0.07</v>
       </c>
       <c r="C6" s="2" t="n">
-        <f aca="false">LN(10)*$B$32*$B$31*B6</f>
+        <f aca="false">LN(10)*$B$33*$B$32*B6</f>
         <v>-392.658950840617</v>
       </c>
       <c r="D6" s="5" t="n">
@@ -550,18 +617,18 @@
         <v>-0.331840136895007</v>
       </c>
       <c r="F6" s="6"/>
-      <c r="G6" s="5"/>
+      <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>-1.05</v>
       </c>
       <c r="C7" s="2" t="n">
-        <f aca="false">LN(10)*$B$32*$B$31*B7</f>
+        <f aca="false">LN(10)*$B$33*$B$32*B7</f>
         <v>-5889.88426260925</v>
       </c>
       <c r="D7" s="5" t="n">
@@ -572,18 +639,18 @@
         <v>-0.0221226757930005</v>
       </c>
       <c r="F7" s="6"/>
-      <c r="G7" s="5"/>
+      <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>0.82</v>
       </c>
       <c r="C8" s="2" t="n">
-        <f aca="false">LN(10)*$B$32*$B$31*B8</f>
+        <f aca="false">LN(10)*$B$33*$B$32*B8</f>
         <v>4599.71913841865</v>
       </c>
       <c r="D8" s="5" t="n">
@@ -594,18 +661,18 @@
         <v>0.0594456585510865</v>
       </c>
       <c r="F8" s="6"/>
-      <c r="G8" s="5"/>
+      <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>-0.39</v>
       </c>
       <c r="C9" s="2" t="n">
-        <f aca="false">LN(10)*$B$32*$B$31*B9</f>
+        <f aca="false">LN(10)*$B$33*$B$32*B9</f>
         <v>-2187.67129754058</v>
       </c>
       <c r="D9" s="5" t="n">
@@ -616,18 +683,18 @@
         <v>-0.124988307722797</v>
       </c>
       <c r="F9" s="6"/>
-      <c r="G9" s="5"/>
+      <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>0.1</v>
       </c>
       <c r="C10" s="2" t="n">
-        <f aca="false">LN(10)*$B$32*$B$31*B10</f>
+        <f aca="false">LN(10)*$B$33*$B$32*B10</f>
         <v>560.941358343738</v>
       </c>
       <c r="D10" s="5" t="n">
@@ -638,18 +705,18 @@
         <v>0.385126413162337</v>
       </c>
       <c r="F10" s="6"/>
-      <c r="G10" s="5"/>
+      <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>0.36</v>
       </c>
       <c r="C11" s="2" t="n">
-        <f aca="false">LN(10)*$B$32*$B$31*B11</f>
+        <f aca="false">LN(10)*$B$33*$B$32*B11</f>
         <v>2019.38889003746</v>
       </c>
       <c r="D11" s="5" t="n">
@@ -660,18 +727,18 @@
         <v>0.106616413045635</v>
       </c>
       <c r="F11" s="6"/>
-      <c r="G11" s="5"/>
+      <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>-0.98</v>
       </c>
       <c r="C12" s="2" t="n">
-        <f aca="false">LN(10)*$B$32*$B$31*B12</f>
+        <f aca="false">LN(10)*$B$33*$B$32*B12</f>
         <v>-5497.22531176863</v>
       </c>
       <c r="D12" s="5" t="n">
@@ -682,18 +749,18 @@
         <v>-0.0391652129555394</v>
       </c>
       <c r="F12" s="6"/>
-      <c r="G12" s="5"/>
+      <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>0</v>
       </c>
       <c r="C13" s="2" t="n">
-        <f aca="false">LN(10)*$B$32*$B$31*B13</f>
+        <f aca="false">LN(10)*$B$33*$B$32*B13</f>
         <v>0</v>
       </c>
       <c r="D13" s="5" t="n">
@@ -701,18 +768,38 @@
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="2"/>
+      <c r="G13" s="2" t="n">
+        <v>0.94</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>1.47</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <f aca="false">G13-$G$13</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="1" t="n">
+        <f aca="false">H13-$H$13</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <f aca="false">I13*$G$32</f>
+        <v>0</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <f aca="false">J13*$G$32</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2" t="n">
         <v>0.39</v>
       </c>
       <c r="C14" s="2" t="n">
-        <f aca="false">LN(10)*$B$32*$B$31*B14</f>
+        <f aca="false">LN(10)*$B$33*$B$32*B14</f>
         <v>2187.67129754058</v>
       </c>
       <c r="D14" s="5" t="n">
@@ -720,21 +807,21 @@
       </c>
       <c r="E14" s="5" t="n">
         <f aca="false">D14/C14</f>
-        <v>0.0925794170088645</v>
+        <v>0.0925794170088646</v>
       </c>
       <c r="F14" s="6"/>
-      <c r="G14" s="5"/>
+      <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B15" s="6" t="n">
         <v>-0.84</v>
       </c>
       <c r="C15" s="2" t="n">
-        <f aca="false">LN(10)*$B$32*$B$31*B15</f>
+        <f aca="false">LN(10)*$B$33*$B$32*B15</f>
         <v>-4711.9074100874</v>
       </c>
       <c r="D15" s="5" t="n">
@@ -745,18 +832,18 @@
         <v>-0.0429833007541157</v>
       </c>
       <c r="F15" s="6"/>
-      <c r="G15" s="5"/>
+      <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B16" s="2" t="n">
         <v>1.55</v>
       </c>
       <c r="C16" s="2" t="n">
-        <f aca="false">LN(10)*$B$32*$B$31*B16</f>
+        <f aca="false">LN(10)*$B$33*$B$32*B16</f>
         <v>8694.59105432794</v>
       </c>
       <c r="D16" s="5" t="n">
@@ -767,20 +854,48 @@
         <v>0.0483595679244016</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>4.92</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>7.7</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <f aca="false">G16-$G$13</f>
+        <v>3.98</v>
+      </c>
+      <c r="J16" s="1" t="n">
+        <f aca="false">H16-$H$13</f>
+        <v>6.23</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <f aca="false">I16*$G$32</f>
+        <v>16509.04</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <f aca="false">J16*$G$32</f>
+        <v>25842.04</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <f aca="false">$D$2/K16</f>
+        <v>0.0108788881727829</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <f aca="false">$D$2/L16</f>
+        <v>0.00694991571872809</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>1.64</v>
       </c>
       <c r="C17" s="2" t="n">
-        <f aca="false">LN(10)*$B$32*$B$31*B17</f>
+        <f aca="false">LN(10)*$B$33*$B$32*B17</f>
         <v>9199.4382768373</v>
       </c>
       <c r="D17" s="5" t="n">
@@ -791,20 +906,48 @@
         <v>0.04361135842502</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>4.92</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>7.85</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <f aca="false">G17-$G$13</f>
+        <v>3.98</v>
+      </c>
+      <c r="J17" s="1" t="n">
+        <f aca="false">H17-$H$13</f>
+        <v>6.38</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <f aca="false">I17*$G$32</f>
+        <v>16509.04</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <f aca="false">J17*$G$32</f>
+        <v>26464.24</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <f aca="false">$D$2/K17</f>
+        <v>0.0108788881727829</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <f aca="false">$D$2/L17</f>
+        <v>0.0067865164463442</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B18" s="2" t="n">
         <v>-0.12</v>
       </c>
       <c r="C18" s="2" t="n">
-        <f aca="false">LN(10)*$B$32*$B$31*B18</f>
+        <f aca="false">LN(10)*$B$33*$B$32*B18</f>
         <v>-673.129630012486</v>
       </c>
       <c r="D18" s="5" t="n">
@@ -815,18 +958,18 @@
         <v>-0.427010371431728</v>
       </c>
       <c r="F18" s="6"/>
-      <c r="G18" s="5"/>
+      <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B19" s="2" t="n">
         <v>-1.14</v>
       </c>
       <c r="C19" s="2" t="n">
-        <f aca="false">LN(10)*$B$32*$B$31*B19</f>
+        <f aca="false">LN(10)*$B$33*$B$32*B19</f>
         <v>-6394.73148511861</v>
       </c>
       <c r="D19" s="5" t="n">
@@ -837,18 +980,18 @@
         <v>-0.0449484601507082</v>
       </c>
       <c r="F19" s="6"/>
-      <c r="G19" s="5"/>
+      <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B20" s="2" t="n">
         <v>1.42</v>
       </c>
       <c r="C20" s="2" t="n">
-        <f aca="false">LN(10)*$B$32*$B$31*B20</f>
+        <f aca="false">LN(10)*$B$33*$B$32*B20</f>
         <v>7965.36728848108</v>
       </c>
       <c r="D20" s="5" t="n">
@@ -859,20 +1002,48 @@
         <v>0.0233971215534752</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>4.86</v>
+      </c>
+      <c r="I20" s="1" t="n">
+        <f aca="false">G20-$G$13</f>
+        <v>1.41</v>
+      </c>
+      <c r="J20" s="1" t="n">
+        <f aca="false">H20-$H$13</f>
+        <v>3.39</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <f aca="false">I20*$G$32</f>
+        <v>5848.68</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <f aca="false">J20*$G$32</f>
+        <v>14061.72</v>
+      </c>
+      <c r="M20" s="0" t="n">
+        <f aca="false">$D$2/K20</f>
+        <v>0.0307077836366496</v>
+      </c>
+      <c r="N20" s="0" t="n">
+        <f aca="false">$D$2/L20</f>
+        <v>0.0127722639904649</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B21" s="2" t="n">
         <v>1.63</v>
       </c>
       <c r="C21" s="2" t="n">
-        <f aca="false">LN(10)*$B$32*$B$31*B21</f>
+        <f aca="false">LN(10)*$B$33*$B$32*B21</f>
         <v>9143.34414100293</v>
       </c>
       <c r="D21" s="5" t="n">
@@ -883,20 +1054,48 @@
         <v>0.043124265467793</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G21" s="5"/>
-      <c r="H21" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="G21" s="2" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="H21" s="2" t="n">
+        <v>5.93</v>
+      </c>
+      <c r="I21" s="1" t="n">
+        <f aca="false">G21-$G$13</f>
+        <v>2.04</v>
+      </c>
+      <c r="J21" s="1" t="n">
+        <f aca="false">H21-$H$13</f>
+        <v>4.46</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <f aca="false">I21*$G$32</f>
+        <v>8461.92</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <f aca="false">J21*$G$32</f>
+        <v>18500.08</v>
+      </c>
+      <c r="M21" s="0" t="n">
+        <f aca="false">$D$2/K21</f>
+        <v>0.0212244975135667</v>
+      </c>
+      <c r="N21" s="0" t="n">
+        <f aca="false">$D$2/L21</f>
+        <v>0.00970806612728161</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B22" s="2" t="n">
         <v>0.77</v>
       </c>
       <c r="C22" s="2" t="n">
-        <f aca="false">LN(10)*$B$32*$B$31*B22</f>
+        <f aca="false">LN(10)*$B$33*$B$32*B22</f>
         <v>4319.24845924678</v>
       </c>
       <c r="D22" s="5" t="n">
@@ -904,22 +1103,22 @@
       </c>
       <c r="E22" s="9" t="n">
         <f aca="false">D22/C22</f>
-        <v>0.0419826122632814</v>
+        <v>0.0419826122632813</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G22" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="G22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B23" s="2" t="n">
         <v>-0.08</v>
       </c>
       <c r="C23" s="2" t="n">
-        <f aca="false">LN(10)*$B$32*$B$31*B23</f>
+        <f aca="false">LN(10)*$B$33*$B$32*B23</f>
         <v>-448.75308667499</v>
       </c>
       <c r="D23" s="5" t="n">
@@ -927,20 +1126,20 @@
       </c>
       <c r="E23" s="5" t="n">
         <f aca="false">D23/C23</f>
-        <v>-0.245049382237031</v>
+        <v>-0.24504938223703</v>
       </c>
       <c r="F23" s="6"/>
-      <c r="G23" s="5"/>
+      <c r="G23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B24" s="2" t="n">
         <v>0.33</v>
       </c>
       <c r="C24" s="2" t="n">
-        <f aca="false">LN(10)*$B$32*$B$31*B24</f>
+        <f aca="false">LN(10)*$B$33*$B$32*B24</f>
         <v>1851.10648253434</v>
       </c>
       <c r="D24" s="5" t="n">
@@ -951,17 +1150,17 @@
         <v>0.112545299419029</v>
       </c>
       <c r="F24" s="6"/>
-      <c r="G24" s="5"/>
+      <c r="G24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B25" s="2" t="n">
         <v>1.14</v>
       </c>
       <c r="C25" s="2" t="n">
-        <f aca="false">LN(10)*$B$32*$B$31*B25</f>
+        <f aca="false">LN(10)*$B$33*$B$32*B25</f>
         <v>6394.73148511861</v>
       </c>
       <c r="D25" s="5" t="n">
@@ -969,22 +1168,51 @@
       </c>
       <c r="E25" s="10" t="n">
         <f aca="false">D25/C25</f>
-        <v>0.073466728211073</v>
+        <v>0.0734667282110729</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G25" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="G25" s="2" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="H25" s="1" t="n">
+        <v>5.73</v>
+      </c>
+      <c r="I25" s="1" t="n">
+        <f aca="false">G25-$G$13</f>
+        <v>1.39</v>
+      </c>
+      <c r="J25" s="1" t="n">
+        <f aca="false">H25-$H$13</f>
+        <v>4.26</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <f aca="false">I25*$G$32</f>
+        <v>5765.72</v>
+      </c>
+      <c r="L25" s="0" t="n">
+        <f aca="false">J25*$G$32</f>
+        <v>17670.48</v>
+      </c>
+      <c r="M25" s="0" t="n">
+        <f aca="false">$D$2/K25</f>
+        <v>0.0311496222501266</v>
+      </c>
+      <c r="N25" s="0" t="n">
+        <f aca="false">$D$2/L25</f>
+        <v>0.0101638438797361</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B26" s="2" t="n">
         <v>0.88</v>
       </c>
       <c r="C26" s="2" t="n">
-        <f aca="false">LN(10)*$B$32*$B$31*B26</f>
+        <f aca="false">LN(10)*$B$33*$B$32*B26</f>
         <v>4936.2839534249</v>
       </c>
       <c r="D26" s="5" t="n">
@@ -992,20 +1220,20 @@
       </c>
       <c r="E26" s="5" t="n">
         <f aca="false">D26/C26</f>
-        <v>0.0650016631324547</v>
+        <v>0.0650016631324548</v>
       </c>
       <c r="F26" s="6"/>
-      <c r="G26" s="5"/>
+      <c r="G26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B27" s="2" t="n">
         <v>1.18</v>
       </c>
       <c r="C27" s="2" t="n">
-        <f aca="false">LN(10)*$B$32*$B$31*B27</f>
+        <f aca="false">LN(10)*$B$33*$B$32*B27</f>
         <v>6619.10802845611</v>
       </c>
       <c r="D27" s="5" t="n">
@@ -1016,18 +1244,46 @@
         <v>0.0496642949352209</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G27" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="G27" s="2" t="n">
+        <v>4.04</v>
+      </c>
+      <c r="H27" s="1" t="n">
+        <v>6.29</v>
+      </c>
+      <c r="I27" s="1" t="n">
+        <f aca="false">G27-$G$13</f>
+        <v>3.1</v>
+      </c>
+      <c r="J27" s="1" t="n">
+        <f aca="false">H27-$H$13</f>
+        <v>4.82</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <f aca="false">I27*$G$32</f>
+        <v>12858.8</v>
+      </c>
+      <c r="L27" s="0" t="n">
+        <f aca="false">J27*$G$32</f>
+        <v>19993.36</v>
+      </c>
+      <c r="M27" s="0" t="n">
+        <f aca="false">$D$2/K27</f>
+        <v>0.0139670886863471</v>
+      </c>
+      <c r="N27" s="0" t="n">
+        <f aca="false">$D$2/L27</f>
+        <v>0.00898298235014025</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="A29" s="0"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -1037,27 +1293,21 @@
       </c>
       <c r="F29" s="6" t="n">
         <f aca="false">E29/2</f>
-        <v>0.0252281229032419</v>
+        <v>0.0252281229032418</v>
       </c>
       <c r="G29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="A30" s="0"/>
       <c r="E30" s="12" t="n">
         <f aca="false">STDEV(E2,E16,E17,E20,E21,E22,E25,E27)</f>
         <v>0.0181837874354137</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="13" t="n">
-        <v>293</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="A31" s="0"/>
+      <c r="E31" s="12"/>
+      <c r="G31" s="0" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1065,8 +1315,45 @@
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="1" t="n">
+      <c r="B32" s="13" t="n">
+        <v>293</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>4148</v>
+      </c>
+      <c r="M32" s="0" t="n">
+        <f aca="false">AVERAGE(M2:M27)</f>
+        <v>0.0240820793864924</v>
+      </c>
+      <c r="N32" s="0" t="n">
+        <f aca="false">AVERAGE(N2:N27)</f>
+        <v>0.0122650171645577</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="1" t="n">
         <v>8.314462</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>